<commit_message>
Mejora de formato Excel TPE5
</commit_message>
<xml_diff>
--- a/TP´s/Evaluables/Unidad 3/ISW_TPE_5_TESTING_EJECUCION_DE_CASOS_DE_PRUEBA.xlsx
+++ b/TP´s/Evaluables/Unidad 3/ISW_TPE_5_TESTING_EJECUCION_DE_CASOS_DE_PRUEBA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr hidePivotFieldList="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8085" tabRatio="679" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8085" tabRatio="679" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="User Story" sheetId="29" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="141">
   <si>
     <t>TC_001</t>
   </si>
@@ -381,9 +381,6 @@
     <t>El usuario logueado msastre tiene permisos para registrar alquileres. Existen puestos disponibles para el período 15/09/17 al 15/10/17. Existe un usuario cargado de nombre Rosa Fernández.</t>
   </si>
   <si>
-    <t>1. El usuario selecciona "Registrar un alquiler de puesto". 2. El usuario ingresa la fecha de inicio 15/09/17 y la fecha de vencimiento 15/10/17. 3. El usuario selecciona tipo de puesto "Techado" y dimensión "10.0". 4. El usuario selecciona la opción "Buscar" dentro del espacio "Seleccione el Periodo". 5. El usuario selecciona el puesto 1 de la grilla. 6. El usuario ingresa el nombre de cliente "Rosa Fernández". 7. El usuario selecciona la opción "Buscar" dentro del espacio "Buscar Cliente". 8. El usuario selecciona la opción "Aceptar". 9. El usuario selecciona la opción "Sí" para registrar. 10. El usuario selecciona la opción "Sí" para imprimir.</t>
-  </si>
-  <si>
     <t>Registro del alquiler sin cliente</t>
   </si>
   <si>
@@ -402,30 +399,9 @@
     <t>El usuario logueado msastre tiene permisos para registrar alquileres. Existen puestos disponibles para el período 15/09/17 al 15/10/17.</t>
   </si>
   <si>
-    <t>1. El usuario selecciona "Registrar un alquiler de puesto". 2. El usuario ingresa la fecha de inicio 15/09/17 y la fecha de vencimiento 15/10/17. 3. El usuario selecciona tipo de puesto "Techado" y dimensión "10.0". 4. El usuario selecciona la opción "Buscar" dentro del espacio "Seleccione el Periodo". 5. El usuario selecciona el puesto 1 de la grilla. 6. El usuario ingresa el nombre de cliente "Rosa Fernández". 7. El usuario selecciona la opción "Aceptar".</t>
-  </si>
-  <si>
-    <t>1. El sistema muestra la pantalla "Registrar un alquiler de puesto". 4. El sistema muestra la grilla con los puestos que coinciden al tipo, dimensión de puesto ingresado y estén disponibles en las fechas ingresadas. 5. El sistema muestra la última medición del medidor del puesto 1. 7. El sistema muestra un mensaje requieriendo que se ingrese un cliente.</t>
-  </si>
-  <si>
     <t>Cliente no ingresado</t>
   </si>
   <si>
-    <t>1. El usuario selecciona "Registrar un alquiler de puesto". 2. El usuario ingresa la fecha de inicio 15/09/17 y la fecha de vencimiento 15/10/17. 3. El usuario selecciona tipo de puesto "Techado" y dimensión "10.0". 4. El usuario selecciona la opción "Buscar" dentro del espacio "Seleccione el Periodo". 5. El usuario ingresa el nombre de cliente "Rosa Fernández". 6. El usuario selecciona la opción "Buscar" dentro del espacio "Buscar Cliente". 7. El usuario selecciona la opción "Aceptar".</t>
-  </si>
-  <si>
-    <t>1. El sistema muestra la pantalla "Registrar un alquiler de puesto". 4. El sistema muestra la grilla con los puestos que coinciden al tipo, dimensión de puesto ingresado y estén disponibles en las fechas ingresadas. 6. El sistema muestra dirección y CUIT de cliente. 7. El sistema muestra un mensaje requiriendo seleccionar un puesto.</t>
-  </si>
-  <si>
-    <t>1. El sistema muestra la pantalla "Registrar un alquiler de puesto". 4. El sistema muestra la grilla con los puestos que coinciden al tipo, dimensión de puesto ingresado y estén disponibles en las fechas ingresadas. 5. El sistema muestra la última medición del medidor del puesto 1. 7. El sistema muestra dirección y CUIT de cliente. 8. El sistema consulta al usuario si confirma el registro. 9. El sistema muestra el número de contrato y consulta si quiere imprimirlo. 10. El sistema imprime el contrato.</t>
-  </si>
-  <si>
-    <t>1. El sistema muestra la pantalla "Registrar un alquiler de puesto". 4. El sistema muestra la grilla con los puestos que coinciden al tipo, dimensión de puesto ingresado y estén disponibles en las fechas ingresadas. 5. El sistema muestra la última medición del medidor del puesto 1. 7. El sistema muestra dirección y CUIT de cliente. 9. El sistema muestra un mensaje alertando que se modificó la fecha después de seleccionar el puesto.</t>
-  </si>
-  <si>
-    <t>1. El usuario selecciona "Registrar un alquiler de puesto". 2. El usuario ingresa la fecha de inicio 15/09/17 y la fecha de vencimiento 15/10/17. 3. El usuario selecciona tipo de puesto "Techado" y dimensión "10.0". 4. El usuario selecciona la opción "Buscar" dentro del espacio "Seleccione el Periodo". 5. El usuario selecciona el puesto 1 de la grilla. 6. El usuario ingresa el nombre de cliente "Rosa Fernández". 7. El usuario selecciona la opción "Buscar" dentro del espacio "Buscar Cliente". 8. El usuario cambia la fecha de inicio por "20/09/2017". 9. El usuario selecciona la opción "Aceptar".</t>
-  </si>
-  <si>
     <t>Formato de fecha de inicio válido</t>
   </si>
   <si>
@@ -478,6 +454,92 @@
   </si>
   <si>
     <t>Media</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona "Registrar un alquiler de puesto". 
+2. El usuario ingresa la fecha de inicio 15/09/17 y la fecha de vencimiento 15/10/17. 
+3. El usuario selecciona tipo de puesto "Techado" y dimensión "10.0". 
+4. El usuario selecciona la opción "Buscar" dentro del espacio "Seleccione el Periodo". 
+5. El usuario selecciona el puesto 1 de la grilla. 6. El usuario ingresa el nombre de cliente "Rosa Fernández". 
+7. El usuario selecciona la opción "Buscar" dentro del espacio "Buscar Cliente". 
+8. El usuario selecciona la opción "Aceptar". 
+9. El usuario selecciona la opción "Sí" para registrar. 
+10. El usuario selecciona la opción "Sí" para imprimir.</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla "Registrar un alquiler de puesto". 
+4. El sistema muestra la grilla con los puestos que coinciden al tipo, dimensión de puesto ingresado y estén disponibles en las fechas ingresadas. 
+5. El sistema muestra la última medición del medidor del puesto 1. 
+7. El sistema muestra dirección y CUIT de cliente. 
+8. El sistema consulta al usuario si confirma el registro. 
+9. El sistema muestra el número de contrato y consulta si quiere imprimirlo. 
+10. El sistema imprime el contrato.</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona "Registrar un alquiler de puesto". 
+2. El usuario ingresa la fecha de inicio 15/09/17 y la fecha de vencimiento 15/10/17. 
+3. El usuario selecciona tipo de puesto "Techado" y dimensión "10.0". 
+4. El usuario selecciona la opción "Buscar" dentro del espacio "Seleccione el Periodo". 
+5. El usuario selecciona el puesto 1 de la grilla. 6. El usuario ingresa el nombre de cliente "Rosa Fernández". 
+7. El usuario selecciona la opción "Aceptar".</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona "Registrar un alquiler de puesto". 
+2. El usuario ingresa la fecha de inicio 15/09/17 y la fecha de vencimiento 15/10/17. 
+3. El usuario selecciona tipo de puesto "Techado" y dimensión "10.0". 
+4. El usuario selecciona la opción "Buscar" dentro del espacio "Seleccione el Periodo". 
+5. El usuario ingresa el nombre de cliente "Rosa Fernández". 
+6. El usuario selecciona la opción "Buscar" dentro del espacio "Buscar Cliente". 
+7. El usuario selecciona la opción "Aceptar".</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona "Registrar un alquiler de puesto". 
+2. El usuario ingresa la fecha de inicio 15/09/17 y la fecha de vencimiento 15/10/17. 
+3. El usuario selecciona tipo de puesto "Techado" y dimensión "10.0". 
+4. El usuario selecciona la opción "Buscar" dentro del espacio "Seleccione el Periodo". 
+5. El usuario selecciona el puesto 1 de la grilla. 6. El usuario ingresa el nombre de cliente "Rosa Fernández". 
+7. El usuario selecciona la opción "Buscar" dentro del espacio "Buscar Cliente". 
+8. El usuario cambia la fecha de inicio por "20/09/2017". 
+9. El usuario selecciona la opción "Aceptar".</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla "Registrar un alquiler de puesto". 
+4. El sistema muestra la grilla con los puestos que coinciden al tipo, dimensión de puesto ingresado y estén disponibles en las fechas ingresadas. 
+5. El sistema muestra la última medición del medidor del puesto 1. 
+7. El sistema muestra un mensaje requieriendo que se ingrese un cliente.</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla "Registrar un alquiler de puesto". 
+4. El sistema muestra la grilla con los puestos que coinciden al tipo, dimensión de puesto ingresado y estén disponibles en las fechas ingresadas. 
+6. El sistema muestra dirección y CUIT de cliente. 
+7. El sistema muestra un mensaje requiriendo seleccionar un puesto.</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla "Registrar un alquiler de puesto". 
+4. El sistema muestra la grilla con los puestos que coinciden al tipo, dimensión de puesto ingresado y estén disponibles en las fechas ingresadas. 
+5. El sistema muestra la última medición del medidor del puesto 1. 
+7. El sistema muestra dirección y CUIT de cliente. 
+9. El sistema muestra un mensaje alertando que se modificó la fecha después de seleccionar el puesto.</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona "Registrar un alquiler de puesto". 
+2. El usuario ingresa la fecha de inicio 15/09/17 y la fecha de vencimiento 15/10/17. 
+3. El usuario selecciona tipo de puesto "Techado" y dimensión "10.0". 
+4. El usuario selecciona la opción "Buscar" dentro del espacio "Seleccione el Periodo". 
+5. El usuario selecciona el puesto 1 de la grilla. 
+6. El usuario ingresa el nombre de cliente "Rosa Fernández". 
+7. El usuario selecciona la opción "Aceptar".</t>
+  </si>
+  <si>
+    <t>1. El usuario selecciona "Registrar un alquiler de puesto". 
+2. El usuario ingresa la fecha de inicio 15/09/17 y la fecha de vencimiento 15/10/17. 
+3. El usuario selecciona tipo de puesto "Techado" y dimensión "10.0". 
+4. El usuario selecciona la opción "Buscar" dentro del espacio "Seleccione el Periodo". 
+5. El usuario selecciona el puesto 1 de la grilla. 
+6. El usuario ingresa el nombre de cliente "Rosa Fernández". 
+7. El usuario selecciona la opción "Buscar" dentro del espacio "Buscar Cliente". 
+8. El usuario cambia la fecha de inicio por "20/09/2017". 
+9. El usuario selecciona la opción "Aceptar".</t>
   </si>
 </sst>
 </file>
@@ -969,7 +1031,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1125,16 +1187,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1150,31 +1209,7 @@
     <cellStyle name="Normal 2 2" xfId="8"/>
     <cellStyle name="Total" xfId="9" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="99">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="51"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="60"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="50"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="68">
     <dxf>
       <fill>
         <patternFill>
@@ -1192,6 +1227,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -1241,6 +1311,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF33CC33"/>
         </patternFill>
       </fill>
@@ -1284,251 +1368,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1964,7 +1803,7 @@
         <xdr:cNvPr id="2" name="Imagen 1" descr="C:\Users\jmele\AppData\Local\Microsoft\Windows\INetCacheContent.Word\Diseño de Interfaces.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0B4D8C93-4A2F-4502-8E43-5732736ADE6B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B4D8C93-4A2F-4502-8E43-5732736ADE6B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2531,16 +2370,17 @@
   </sheetPr>
   <dimension ref="A1:AS73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="10" style="2" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.85546875" style="9" customWidth="1"/>
     <col min="6" max="6" width="38.140625" style="11" customWidth="1"/>
     <col min="7" max="7" width="52" style="12" customWidth="1"/>
@@ -2702,11 +2542,11 @@
       </c>
       <c r="B5" s="61"/>
       <c r="C5" s="43"/>
-      <c r="D5" s="66" t="s">
-        <v>137</v>
-      </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="64"/>
+      <c r="D5" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="64"/>
+      <c r="F5" s="65"/>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
@@ -2885,7 +2725,7 @@
       <c r="AB10" s="6"/>
       <c r="AL10" s="6"/>
     </row>
-    <row r="11" spans="1:45" ht="180" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" ht="216" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>0</v>
       </c>
@@ -2893,7 +2733,7 @@
         <v>103</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" s="27" t="s">
         <v>104</v>
@@ -2902,22 +2742,22 @@
         <v>105</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="G11" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="H11" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="H11" s="65" t="s">
-        <v>126</v>
-      </c>
       <c r="I11" s="15" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="J11" s="37" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="K11" s="37" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="L11" s="37">
         <v>42990</v>
@@ -2939,36 +2779,36 @@
       <c r="AR11" s="7"/>
       <c r="AS11" s="7"/>
     </row>
-    <row r="12" spans="1:45" ht="132" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" ht="144" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>112</v>
-      </c>
       <c r="F12" s="26" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="H12" s="65" t="s">
-        <v>127</v>
+        <v>136</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>119</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="J12" s="28" t="s">
-        <v>128</v>
+        <v>116</v>
+      </c>
+      <c r="J12" s="26" t="s">
+        <v>120</v>
       </c>
       <c r="K12" s="29">
         <v>1</v>
@@ -2993,36 +2833,36 @@
       <c r="AR12" s="7"/>
       <c r="AS12" s="7"/>
     </row>
-    <row r="13" spans="1:45" ht="132" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" ht="156" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>112</v>
-      </c>
       <c r="F13" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="G13" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="H13" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="J13" s="28" t="s">
-        <v>129</v>
+      <c r="J13" s="26" t="s">
+        <v>121</v>
       </c>
       <c r="K13" s="29">
         <v>2</v>
@@ -3047,7 +2887,7 @@
       <c r="AR13" s="7"/>
       <c r="AS13" s="7"/>
     </row>
-    <row r="14" spans="1:45" ht="168" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" ht="192" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>42</v>
       </c>
@@ -3055,28 +2895,28 @@
         <v>103</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="H14" s="65" t="s">
-        <v>126</v>
+        <v>138</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>118</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="J14" s="28" t="s">
-        <v>130</v>
+        <v>116</v>
+      </c>
+      <c r="J14" s="26" t="s">
+        <v>122</v>
       </c>
       <c r="K14" s="29">
         <v>3</v>
@@ -3113,7 +2953,7 @@
       <c r="G15" s="26"/>
       <c r="H15" s="26"/>
       <c r="I15" s="15"/>
-      <c r="J15" s="28"/>
+      <c r="J15" s="26"/>
       <c r="K15" s="29"/>
       <c r="L15" s="37"/>
       <c r="M15" s="39"/>
@@ -3145,7 +2985,7 @@
       <c r="G16" s="26"/>
       <c r="H16" s="26"/>
       <c r="I16" s="15"/>
-      <c r="J16" s="28"/>
+      <c r="J16" s="26"/>
       <c r="K16" s="29"/>
       <c r="L16" s="37"/>
       <c r="M16" s="39"/>
@@ -5000,247 +4840,247 @@
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="D5:F5"/>
   </mergeCells>
-  <conditionalFormatting sqref="J623:J747 J749 J751 J753 J755 J757 J759 J761 J763 J765:J771 J919:J1042 J1044:J1181 J1186:J1200 J1205:J1209 J1214:J1263 J1267:J1291 J1293:J1385 J1389:J1413 J1415:J1474 J1476:J1562 J1601:J1622 J1759:J1760 J1763:J1790 J1918:J1959 J1962:J1964 J1967 J1969:J1971 J1974:J2011 J2014:J2054 J2057:J2079 J2082:J2085 J2088 J2090:J2092 J2095:J2136 J2332:J65044 J9:J10 O623:O747 O749 O751 O753 O755 O757 O759 O761 O763 O765:O771 O919:O1042 O1044:O1181 O1186:O1200 O1205:O1209 O1214:O1263 O1267:O1291 O1293:O1385 O1389:O1413 O1415:O1474 O1476:O1562 O1601:O1622 O1759:O1760 O1763:O1790 O1918:O1959 O1962:O1964 O1967 O1969:O1971 O1974:O2011 O2014:O2054 O2057:O2079 O2082:O2085 O2088 O2090:O2092 O2095:O2136 O2332:O65044 O9:O10 O12:O606 J12:J606">
-    <cfRule type="cellIs" dxfId="98" priority="89" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="J623:J747 J749 J751 J753 J755 J757 J759 J761 J763 J765:J771 J919:J1042 J1044:J1181 J1186:J1200 J1205:J1209 J1214:J1263 J1267:J1291 J1293:J1385 J1389:J1413 J1415:J1474 J1476:J1562 J1601:J1622 J1759:J1760 J1763:J1790 J1918:J1959 J1962:J1964 J1967 J1969:J1971 J1974:J2011 J2014:J2054 J2057:J2079 J2082:J2085 J2088 J2090:J2092 J2095:J2136 J2332:J65044 J9:J10 O623:O747 O749 O751 O753 O755 O757 O759 O761 O763 O765:O771 O919:O1042 O1044:O1181 O1186:O1200 O1205:O1209 O1214:O1263 O1267:O1291 O1293:O1385 O1389:O1413 O1415:O1474 O1476:O1562 O1601:O1622 O1759:O1760 O1763:O1790 O1918:O1959 O1962:O1964 O1967 O1969:O1971 O1974:O2011 O2014:O2054 O2057:O2079 O2082:O2085 O2088 O2090:O2092 O2095:O2136 O2332:O65044 O9:O10 O12:O606 J17:J606">
+    <cfRule type="cellIs" dxfId="67" priority="89" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="90" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="90" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="91" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="91" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:I73 N12:N73">
-    <cfRule type="cellIs" dxfId="95" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="81" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="82" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="83" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="84" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="85" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:I73 N12:N73">
-    <cfRule type="cellIs" dxfId="90" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="66" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="67" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T623:T747 T749 T751 T753 T755 T757 T759 T761 T763 T765:T771 T919:T1042 T1044:T1181 T1186:T1200 T1205:T1209 T1214:T1263 T1267:T1291 T1293:T1385 T1389:T1413 T1415:T1474 T1476:T1562 T1601:T1622 T1759:T1760 T1763:T1790 T1918:T1959 T1962:T1964 T1967 T1969:T1971 T1974:T2011 T2014:T2054 T2057:T2079 T2082:T2085 T2088 T2090:T2092 T2095:T2136 T2332:T65044 T9:T10 T12:T606">
-    <cfRule type="cellIs" dxfId="88" priority="56" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="56" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="57" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="57" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="58" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="58" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S12:S73">
-    <cfRule type="cellIs" dxfId="85" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="51" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="52" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="54" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="55" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S12:S73">
-    <cfRule type="cellIs" dxfId="80" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="cellIs" dxfId="78" priority="46" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="46" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="47" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="47" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="48" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="75" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="41" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="42" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="44" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="45" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="70" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S11">
-    <cfRule type="cellIs" dxfId="68" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="36" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="37" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="38" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="38" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R11">
-    <cfRule type="cellIs" dxfId="65" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="31" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="32" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="35" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R11">
-    <cfRule type="cellIs" dxfId="60" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="58" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="24" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="48" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="44" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="17" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="21" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="34" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5263,7 +5103,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5320,7 +5162,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
         <v>1</v>
       </c>
@@ -5331,22 +5173,22 @@
         <v>42990</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>103</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="120" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="156" x14ac:dyDescent="0.2">
       <c r="A5" s="20">
         <v>2</v>
       </c>
@@ -5357,22 +5199,22 @@
         <v>42990</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G5" s="21" t="s">
         <v>103</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A6" s="20">
         <v>3</v>
       </c>
@@ -5383,19 +5225,19 @@
         <v>42990</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -5565,14 +5407,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -5698,6 +5532,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
   <ds:schemaRefs>
@@ -5707,22 +5549,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5738,4 +5564,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>